<commit_message>
updated BOM and changed 2 pin conns to 3 pins
</commit_message>
<xml_diff>
--- a/dwg/roboCoolerBOM.xlsx
+++ b/dwg/roboCoolerBOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
   <si>
     <t>Item</t>
   </si>
@@ -63,16 +63,61 @@
     <t>Total Cost</t>
   </si>
   <si>
-    <t>TI</t>
-  </si>
-  <si>
-    <t>SN74AC14N</t>
-  </si>
-  <si>
-    <t>Inverters Hex Schmitt-Trigger</t>
-  </si>
-  <si>
-    <t>595-SN74AC14N</t>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>P1 P2</t>
+  </si>
+  <si>
+    <t>Sparkfun</t>
+  </si>
+  <si>
+    <t>BOB-00717</t>
+  </si>
+  <si>
+    <t>SOT23 to DIP adapter</t>
+  </si>
+  <si>
+    <t>Ti</t>
+  </si>
+  <si>
+    <t>SN74LVC1G04QDBVRQ1</t>
+  </si>
+  <si>
+    <t>IC SINGLE INVERTER GATE SOT23-5</t>
+  </si>
+  <si>
+    <t>FQPF13N06L</t>
+  </si>
+  <si>
+    <t>FQPF11P06</t>
+  </si>
+  <si>
+    <t>Fairchild</t>
+  </si>
+  <si>
+    <t>MOSFET N-CH 60V 10A TO-220F</t>
+  </si>
+  <si>
+    <t>MOSFET P-CH 60V 8.6A TO-220F</t>
+  </si>
+  <si>
+    <t>Q1 Q5</t>
+  </si>
+  <si>
+    <t>Q2 Q3 Q4 Q6</t>
+  </si>
+  <si>
+    <t>Vishay</t>
+  </si>
+  <si>
+    <t>BAT42-TR</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 30V 200MA DO35</t>
+  </si>
+  <si>
+    <t>D1 D2 D3 D4 D5 D6</t>
   </si>
 </sst>
 </file>
@@ -80,9 +125,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,50 +157,122 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8F8F8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -167,23 +284,48 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -481,259 +623,396 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="7">
+      <c r="K1" s="8">
         <f>SUM(J2:J100)</f>
-        <v>6.25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="2" customFormat="1">
-      <c r="A2" s="2">
+        <v>15.61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="15" customHeight="1">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="2">
+      <c r="E2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="9">
         <v>2</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="11">
         <v>2.89</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2" s="11">
         <f>I2*F2</f>
         <v>5.78</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" s="6" customFormat="1">
-      <c r="A3" s="6">
+      <c r="K2" s="13"/>
+    </row>
+    <row r="3" spans="1:11" s="3" customFormat="1" ht="28.5">
+      <c r="A3" s="9">
+        <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="11" t="s">
+      <c r="F3" s="9">
+        <v>1</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="11">
+        <v>0.48</v>
+      </c>
+      <c r="J3" s="11">
+        <f>I3*F3</f>
+        <v>0.48</v>
+      </c>
+      <c r="K3" s="13"/>
+    </row>
+    <row r="4" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="A4" s="9">
+        <f>A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="6">
+      <c r="C4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="9">
         <v>1</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="11">
+        <v>0.95</v>
+      </c>
+      <c r="J4" s="11">
+        <f>I4*F4</f>
+        <v>0.95</v>
+      </c>
+      <c r="K4" s="13"/>
+    </row>
+    <row r="5" spans="1:11" ht="28.5">
+      <c r="A5" s="9">
+        <f>A4+1</f>
+        <v>4</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="14">
+        <v>4</v>
+      </c>
+      <c r="G5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="7">
-        <v>0.47</v>
-      </c>
-      <c r="J3" s="8">
-        <f>I3*F3</f>
-        <v>0.47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
+      <c r="H5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="15">
+        <v>0.89</v>
+      </c>
+      <c r="J5" s="11">
+        <f>I5*F5</f>
+        <v>3.56</v>
+      </c>
+      <c r="K5" s="13"/>
+    </row>
+    <row r="6" spans="1:11" ht="28.5">
+      <c r="A6" s="9">
+        <f>A5+1</f>
+        <v>5</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="14">
+        <v>2</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J6" s="11">
+        <f>I6*F6</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K6" s="13"/>
+    </row>
+    <row r="7" spans="1:11" ht="42.75">
+      <c r="A7" s="9">
+        <f>A6+1</f>
+        <v>6</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="14">
+        <v>6</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="15">
+        <v>0.44</v>
+      </c>
+      <c r="J7" s="11">
+        <f>I7*F7</f>
+        <v>2.64</v>
+      </c>
+      <c r="K7" s="13"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
     </row>
     <row r="17" spans="9:10">
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
     </row>
     <row r="18" spans="9:10">
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
     </row>
     <row r="19" spans="9:10">
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
     </row>
     <row r="20" spans="9:10">
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
     </row>
     <row r="21" spans="9:10">
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
     </row>
     <row r="22" spans="9:10">
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
     </row>
     <row r="23" spans="9:10">
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
     </row>
     <row r="24" spans="9:10">
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
     </row>
     <row r="25" spans="9:10">
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
     </row>
     <row r="26" spans="9:10">
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
     </row>
     <row r="27" spans="9:10">
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
     </row>
     <row r="28" spans="9:10">
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
     </row>
     <row r="29" spans="9:10">
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
     </row>
     <row r="30" spans="9:10">
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
     </row>
     <row r="31" spans="9:10">
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
     </row>
     <row r="32" spans="9:10">
-      <c r="I32" s="9"/>
-      <c r="J32" s="9"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
     </row>
     <row r="33" spans="9:10">
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
     </row>
     <row r="34" spans="9:10">
-      <c r="I34" s="9"/>
-      <c r="J34" s="9"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
     </row>
     <row r="35" spans="9:10">
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
     </row>
     <row r="36" spans="9:10">
-      <c r="I36" s="9"/>
-      <c r="J36" s="9"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="H3" r:id="rId2"/>
+    <hyperlink ref="H4" r:id="rId2"/>
+    <hyperlink ref="H3" r:id="rId3" location="_"/>
+    <hyperlink ref="H5" r:id="rId4"/>
+    <hyperlink ref="H6" r:id="rId5"/>
+    <hyperlink ref="H7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added connectors to BOM
</commit_message>
<xml_diff>
--- a/dwg/roboCoolerBOM.xlsx
+++ b/dwg/roboCoolerBOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="103">
   <si>
     <t>Item</t>
   </si>
@@ -48,18 +48,6 @@
     <t>3M</t>
   </si>
   <si>
-    <t>6850-4500PL</t>
-  </si>
-  <si>
-    <t>Mouser</t>
-  </si>
-  <si>
-    <t>517-6850-4500PL</t>
-  </si>
-  <si>
-    <t>50 Pin F Header .1"</t>
-  </si>
-  <si>
     <t>Total Cost</t>
   </si>
   <si>
@@ -118,6 +106,225 @@
   </si>
   <si>
     <t>D1 D2 D3 D4 D5 D6</t>
+  </si>
+  <si>
+    <t>1k Resistor</t>
+  </si>
+  <si>
+    <t>K847PH</t>
+  </si>
+  <si>
+    <t>OPTOISOLTR 5KV 4CH TRANS 16-DIP</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>R1 R6 R7 R10 R11</t>
+  </si>
+  <si>
+    <t>100 Ohm Resistor</t>
+  </si>
+  <si>
+    <t>R4 R5 R8 R9</t>
+  </si>
+  <si>
+    <t>M20-9760246</t>
+  </si>
+  <si>
+    <t>Sullins</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PPPC022LJBN-RC</t>
+  </si>
+  <si>
+    <t>4 Position Header Connector 0.100" (2.54mm) Through Hole, Right Angle Gold</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> S5555-ND</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>Harwin</t>
+  </si>
+  <si>
+    <t>02+02 DIL VERT PIN HDR</t>
+  </si>
+  <si>
+    <t>952-1772-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> M20-1070200</t>
+  </si>
+  <si>
+    <t>DIL FEMALE CRIMP HOUSING 2X2POS</t>
+  </si>
+  <si>
+    <t>952-2030-ND</t>
+  </si>
+  <si>
+    <t>FEMALE CRIMP CONTACT TIN LOOSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 952-2159-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> M20-1180046</t>
+  </si>
+  <si>
+    <t>FCI</t>
+  </si>
+  <si>
+    <t>68021-404HLF</t>
+  </si>
+  <si>
+    <t>CONN HEADER 4POS .100 R/A TIN</t>
+  </si>
+  <si>
+    <t>J13 J15</t>
+  </si>
+  <si>
+    <t>609-3351-ND</t>
+  </si>
+  <si>
+    <t>J11</t>
+  </si>
+  <si>
+    <t>P11</t>
+  </si>
+  <si>
+    <t>535677-5</t>
+  </si>
+  <si>
+    <t>TE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2 Position Receptacle Connector 0.100" (2.54mm) Through Hole, Right Angle Tin-Lead</t>
+  </si>
+  <si>
+    <t>A115382-ND</t>
+  </si>
+  <si>
+    <t>961102-6404-AR</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT SGL 2POS GOLD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3M9447-ND</t>
+  </si>
+  <si>
+    <t>M20-1060200</t>
+  </si>
+  <si>
+    <t>SIL FEMALE CRIMP HOUSING 2POS</t>
+  </si>
+  <si>
+    <t>952-2227-ND</t>
+  </si>
+  <si>
+    <t>77311-118-02LF</t>
+  </si>
+  <si>
+    <t>CONN HEADER 2POS VERT T/H</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 609-4434-ND</t>
+  </si>
+  <si>
+    <t>J3 J12 J14</t>
+  </si>
+  <si>
+    <t>P3 P12 P14</t>
+  </si>
+  <si>
+    <t>P4 P13 P15</t>
+  </si>
+  <si>
+    <t>P4 P6 P8 P13 P15</t>
+  </si>
+  <si>
+    <t>929836-01-02-RK</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CONN HEADER 4POS DUAL .100 TIN</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>929836E-01-02-ND</t>
+  </si>
+  <si>
+    <t>J5 J7 J16</t>
+  </si>
+  <si>
+    <t>P5 P7 P16</t>
+  </si>
+  <si>
+    <t>P6 P8 P17</t>
+  </si>
+  <si>
+    <t>J6 J8 J17</t>
+  </si>
+  <si>
+    <t>PPTC121LGBN-RC</t>
+  </si>
+  <si>
+    <t>12 Position Header Connector 0.100" (2.54mm) Through Hole, Right Angle Tin</t>
+  </si>
+  <si>
+    <t>S5448-ND</t>
+  </si>
+  <si>
+    <t>68002-412HLF</t>
+  </si>
+  <si>
+    <t>CONN HEADER 12POS .100 STR TIN</t>
+  </si>
+  <si>
+    <t>609-3308-ND</t>
+  </si>
+  <si>
+    <t>C &amp; K Components</t>
+  </si>
+  <si>
+    <t>D6C90 F1 LFS</t>
+  </si>
+  <si>
+    <t>SWITCH PUSH SPST-NO 0.1A 32V</t>
+  </si>
+  <si>
+    <t>SW1 SW2</t>
+  </si>
+  <si>
+    <t>SFH11-PBPC-D25-ST-BK</t>
+  </si>
+  <si>
+    <t>50 Position Header Connector 0.100" (2.54mm) Through Hole Gold</t>
+  </si>
+  <si>
+    <t>S9201-ND</t>
+  </si>
+  <si>
+    <t>K847PH-ND</t>
+  </si>
+  <si>
+    <t>BAT42CT-ND</t>
+  </si>
+  <si>
+    <t>FQPF11P06FS-ND</t>
+  </si>
+  <si>
+    <t>FQPF13N06L-ND</t>
+  </si>
+  <si>
+    <t>1568-1098-ND</t>
+  </si>
+  <si>
+    <t>296-26588-1-ND</t>
   </si>
 </sst>
 </file>
@@ -185,18 +392,12 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF8F8F8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -223,9 +424,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -233,6 +432,19 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -247,7 +459,9 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -260,20 +474,9 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -284,24 +487,12 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -323,7 +514,20 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -623,366 +827,833 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.28515625" customWidth="1"/>
     <col min="6" max="6" width="6.28515625" customWidth="1"/>
     <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="12">
+        <f>SUM(J2:J100)</f>
+        <v>31.229999999999997</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="3" customFormat="1" ht="28.5">
+      <c r="A2" s="14">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="14">
+        <v>1</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" s="15">
+        <v>0.49</v>
+      </c>
+      <c r="J2" s="15">
+        <f t="shared" ref="J2:J6" si="0">I2*F2</f>
+        <v>0.49</v>
+      </c>
+      <c r="K2" s="9"/>
+    </row>
+    <row r="3" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="A3" s="5">
+        <f t="shared" ref="A3:A23" si="1">A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="8">
-        <f>SUM(J2:J100)</f>
-        <v>17.39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="9">
+      <c r="D3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="9">
-        <v>2</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="11">
-        <v>2.89</v>
-      </c>
-      <c r="J2" s="11">
-        <f t="shared" ref="J2:J7" si="0">I2*F2</f>
-        <v>5.78</v>
-      </c>
-      <c r="K2" s="13"/>
-    </row>
-    <row r="3" spans="1:11" s="3" customFormat="1" ht="28.5">
-      <c r="A3" s="9">
-        <f>A2+1</f>
-        <v>2</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="9">
-        <v>1</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="11">
-        <v>0.48</v>
-      </c>
-      <c r="J3" s="11">
-        <f t="shared" si="0"/>
-        <v>0.48</v>
-      </c>
-      <c r="K3" s="13"/>
-    </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A4" s="9">
-        <f>A3+1</f>
-        <v>3</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="9">
-        <v>1</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="11">
+      <c r="G3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="I3" s="7">
         <v>0.95</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J3" s="7">
         <f t="shared" si="0"/>
         <v>0.95</v>
       </c>
-      <c r="K4" s="13"/>
+      <c r="K3" s="9"/>
+    </row>
+    <row r="4" spans="1:11" ht="28.5">
+      <c r="A4" s="5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="10">
+        <v>6</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="I4" s="11">
+        <v>0.84</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="0"/>
+        <v>5.04</v>
+      </c>
+      <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" ht="28.5">
-      <c r="A5" s="9">
-        <f>A4+1</f>
+      <c r="A5" s="5">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="14" t="s">
+      <c r="B5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="E5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="10">
+        <v>2</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="I5" s="11">
+        <v>1.04</v>
+      </c>
+      <c r="J5" s="7">
+        <f t="shared" si="0"/>
+        <v>2.08</v>
+      </c>
+      <c r="K5" s="9"/>
+    </row>
+    <row r="6" spans="1:11" ht="42.75">
+      <c r="A6" s="5">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="C6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F6" s="10">
         <v>6</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="I6" s="11">
+        <v>0.39</v>
+      </c>
+      <c r="J6" s="7">
+        <f t="shared" si="0"/>
+        <v>2.34</v>
+      </c>
+      <c r="K6" s="9"/>
+    </row>
+    <row r="7" spans="1:11" ht="28.5">
+      <c r="A7" s="5">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="10">
+        <v>1</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="I7" s="11">
+        <v>1.64</v>
+      </c>
+      <c r="J7" s="7">
+        <f t="shared" ref="J7" si="2">I7*F7</f>
+        <v>1.64</v>
+      </c>
+      <c r="K7" s="9"/>
+    </row>
+    <row r="8" spans="1:11" s="2" customFormat="1" ht="57">
+      <c r="A8" s="5">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="5">
+        <v>2</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="I8" s="7">
+        <v>2.89</v>
+      </c>
+      <c r="J8" s="7">
+        <f>I8*F8</f>
+        <v>5.78</v>
+      </c>
+      <c r="K8" s="9"/>
+    </row>
+    <row r="9" spans="1:11" s="2" customFormat="1" ht="57">
+      <c r="A9" s="5">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="5">
+        <v>3</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="J9" s="7">
+        <f>I9*F9</f>
+        <v>2.7</v>
+      </c>
+      <c r="K9" s="9"/>
+    </row>
+    <row r="10" spans="1:11" s="2" customFormat="1" ht="28.5">
+      <c r="A10" s="5">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="5">
+        <v>3</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="J10" s="7">
+        <f>I10*F10</f>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="K10" s="9"/>
+    </row>
+    <row r="11" spans="1:11" s="2" customFormat="1" ht="28.5">
+      <c r="A11" s="5">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" s="5">
+        <v>3</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" s="7">
+        <v>0.18</v>
+      </c>
+      <c r="J11" s="7">
+        <f>I11*F11</f>
+        <v>0.54</v>
+      </c>
+      <c r="K11" s="9"/>
+    </row>
+    <row r="12" spans="1:11" s="2" customFormat="1" ht="42.75">
+      <c r="A12" s="5">
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="H5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="15">
-        <v>0.89</v>
-      </c>
-      <c r="J5" s="11">
-        <f t="shared" si="0"/>
-        <v>5.34</v>
-      </c>
-      <c r="K5" s="13"/>
-    </row>
-    <row r="6" spans="1:11" ht="28.5">
-      <c r="A6" s="9">
-        <f>A5+1</f>
+      <c r="B12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" s="5">
+        <f>F11*4 + F16*2</f>
+        <v>18</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I12" s="7">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J12" s="7">
+        <f>I12*F12</f>
+        <v>2.5200000000000005</v>
+      </c>
+      <c r="K12" s="9"/>
+    </row>
+    <row r="13" spans="1:11" s="2" customFormat="1" ht="28.5">
+      <c r="A13" s="5">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="5">
+        <v>2</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I13" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="J13" s="7">
+        <f>I13*F13</f>
+        <v>0.42</v>
+      </c>
+      <c r="K13" s="9"/>
+    </row>
+    <row r="14" spans="1:11" s="2" customFormat="1" ht="71.25">
+      <c r="A14" s="5">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="5">
+        <v>3</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="I14" s="7">
+        <v>0.33</v>
+      </c>
+      <c r="J14" s="7">
+        <f>I14*F14</f>
+        <v>0.99</v>
+      </c>
+      <c r="K14" s="9"/>
+    </row>
+    <row r="15" spans="1:11" s="2" customFormat="1" ht="28.5">
+      <c r="A15" s="5">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" s="5">
+        <v>3</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15" s="7">
+        <v>0.16</v>
+      </c>
+      <c r="J15" s="7">
+        <f>I15*F15</f>
+        <v>0.48</v>
+      </c>
+      <c r="K15" s="9"/>
+    </row>
+    <row r="16" spans="1:11" s="2" customFormat="1" ht="28.5">
+      <c r="A16" s="5">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" s="5">
+        <v>3</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="I16" s="7">
+        <v>0.13</v>
+      </c>
+      <c r="J16" s="7">
+        <f>I16*F16</f>
+        <v>0.39</v>
+      </c>
+      <c r="K16" s="9"/>
+    </row>
+    <row r="17" spans="1:11" s="2" customFormat="1" ht="28.5">
+      <c r="A17" s="5">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="5">
+        <v>3</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="I17" s="7">
+        <v>0.18</v>
+      </c>
+      <c r="J17" s="7">
+        <f>I17*F17</f>
+        <v>0.54</v>
+      </c>
+      <c r="K17" s="9"/>
+    </row>
+    <row r="18" spans="1:11" s="2" customFormat="1" ht="28.5">
+      <c r="A18" s="5">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="5">
+        <v>1</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I18" s="7">
+        <v>0.65</v>
+      </c>
+      <c r="J18" s="7">
+        <f>I18*F18</f>
+        <v>0.65</v>
+      </c>
+      <c r="K18" s="9"/>
+    </row>
+    <row r="19" spans="1:11" ht="57">
+      <c r="A19" s="5">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="8">
+        <v>1</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="I19" s="13">
+        <v>0.99</v>
+      </c>
+      <c r="J19" s="13">
+        <f>I19*F19</f>
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="28.5">
+      <c r="A20" s="5">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="8">
+        <v>1</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="I20" s="13">
+        <v>0.45</v>
+      </c>
+      <c r="J20" s="13">
+        <f>I20*F20</f>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="28.5">
+      <c r="A21" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F21" s="8">
+        <v>2</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="I21" s="13">
+        <v>0.82</v>
+      </c>
+      <c r="J21" s="13">
+        <f>I21*F21</f>
+        <v>1.64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="42.75">
+      <c r="A22" s="5">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" s="10">
         <v>5</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="14">
-        <v>2</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6" s="15">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J6" s="11">
-        <f t="shared" si="0"/>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="K6" s="13"/>
-    </row>
-    <row r="7" spans="1:11" ht="42.75">
-      <c r="A7" s="9">
-        <f>A6+1</f>
-        <v>6</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="14">
-        <v>6</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" s="15">
-        <v>0.44</v>
-      </c>
-      <c r="J7" s="11">
-        <f t="shared" si="0"/>
-        <v>2.64</v>
-      </c>
-      <c r="K7" s="13"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="9:10">
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="9:10">
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-    </row>
-    <row r="19" spans="9:10">
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-    </row>
-    <row r="20" spans="9:10">
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-    </row>
-    <row r="21" spans="9:10">
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-    </row>
-    <row r="22" spans="9:10">
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-    </row>
-    <row r="23" spans="9:10">
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-    </row>
-    <row r="24" spans="9:10">
+      <c r="G22" s="8"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="7"/>
+    </row>
+    <row r="23" spans="1:11" ht="28.5">
+      <c r="A23" s="5">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="10">
+        <v>4</v>
+      </c>
+      <c r="G23" s="8"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="7"/>
+    </row>
+    <row r="24" spans="1:11">
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
     </row>
-    <row r="25" spans="9:10">
+    <row r="25" spans="1:11">
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
     </row>
-    <row r="26" spans="9:10">
+    <row r="26" spans="1:11">
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
     </row>
-    <row r="27" spans="9:10">
+    <row r="27" spans="1:11">
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
     </row>
-    <row r="28" spans="9:10">
+    <row r="28" spans="1:11">
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
     </row>
-    <row r="29" spans="9:10">
+    <row r="29" spans="1:11">
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
     </row>
-    <row r="30" spans="9:10">
+    <row r="30" spans="1:11">
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
     </row>
-    <row r="31" spans="9:10">
+    <row r="31" spans="1:11">
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
     </row>
-    <row r="32" spans="9:10">
+    <row r="32" spans="1:11">
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
     </row>
@@ -1004,15 +1675,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="H4" r:id="rId2"/>
-    <hyperlink ref="H3" r:id="rId3" location="_"/>
-    <hyperlink ref="H5" r:id="rId4"/>
-    <hyperlink ref="H6" r:id="rId5"/>
-    <hyperlink ref="H7" r:id="rId6"/>
+    <hyperlink ref="H9" r:id="rId1"/>
+    <hyperlink ref="H10" r:id="rId2"/>
+    <hyperlink ref="H11" r:id="rId3"/>
+    <hyperlink ref="H12" r:id="rId4"/>
+    <hyperlink ref="H13" r:id="rId5"/>
+    <hyperlink ref="H14" r:id="rId6"/>
+    <hyperlink ref="H15" r:id="rId7"/>
+    <hyperlink ref="H16" r:id="rId8"/>
+    <hyperlink ref="H17" r:id="rId9"/>
+    <hyperlink ref="H18" r:id="rId10"/>
+    <hyperlink ref="H19" r:id="rId11"/>
+    <hyperlink ref="H20" r:id="rId12"/>
+    <hyperlink ref="H21" r:id="rId13"/>
+    <hyperlink ref="H8" r:id="rId14"/>
+    <hyperlink ref="H7" r:id="rId15"/>
+    <hyperlink ref="H6" r:id="rId16"/>
+    <hyperlink ref="H5" r:id="rId17"/>
+    <hyperlink ref="H4" r:id="rId18"/>
+    <hyperlink ref="H3" r:id="rId19"/>
+    <hyperlink ref="H2" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId21"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
consolidated BOM and fixed some errors before ordering.
</commit_message>
<xml_diff>
--- a/dwg/roboCoolerBOM.xlsx
+++ b/dwg/roboCoolerBOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="96">
   <si>
     <t>Item</t>
   </si>
@@ -225,51 +225,21 @@
     <t>952-2227-ND</t>
   </si>
   <si>
-    <t>77311-118-02LF</t>
-  </si>
-  <si>
-    <t>CONN HEADER 2POS VERT T/H</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 609-4434-ND</t>
-  </si>
-  <si>
     <t>J3 J12 J14</t>
   </si>
   <si>
-    <t>P3 P12 P14</t>
-  </si>
-  <si>
     <t>P4 P13 P15</t>
   </si>
   <si>
     <t>P4 P6 P8 P13 P15</t>
   </si>
   <si>
-    <t>929836-01-02-RK</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CONN HEADER 4POS DUAL .100 TIN</t>
-  </si>
-  <si>
-    <t>J4</t>
-  </si>
-  <si>
-    <t>929836E-01-02-ND</t>
-  </si>
-  <si>
     <t>J5 J7 J16</t>
   </si>
   <si>
-    <t>P5 P7 P16</t>
-  </si>
-  <si>
     <t>P6 P8 P17</t>
   </si>
   <si>
-    <t>J6 J8 J17</t>
-  </si>
-  <si>
     <t>PPTC121LGBN-RC</t>
   </si>
   <si>
@@ -325,6 +295,15 @@
   </si>
   <si>
     <t>296-26588-1-ND</t>
+  </si>
+  <si>
+    <t>P5 P7 P16 J6 J8 J17</t>
+  </si>
+  <si>
+    <t>401-1969-ND</t>
+  </si>
+  <si>
+    <t>P3  J4 P12 P14</t>
   </si>
 </sst>
 </file>
@@ -825,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -878,8 +857,8 @@
         <v>10</v>
       </c>
       <c r="K1" s="12">
-        <f>SUM(J2:J100)</f>
-        <v>31.229999999999997</v>
+        <f>SUM(J2:J98)</f>
+        <v>30.72</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" ht="28.5">
@@ -905,7 +884,7 @@
         <v>42</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="I2" s="15">
         <v>0.49</v>
@@ -918,7 +897,7 @@
     </row>
     <row r="3" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="5">
-        <f t="shared" ref="A3:A23" si="1">A2+1</f>
+        <f t="shared" ref="A3:A21" si="1">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -940,7 +919,7 @@
         <v>42</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="I3" s="7">
         <v>0.95</v>
@@ -975,7 +954,7 @@
         <v>42</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="I4" s="11">
         <v>0.84</v>
@@ -1010,7 +989,7 @@
         <v>42</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="I5" s="11">
         <v>1.04</v>
@@ -1045,7 +1024,7 @@
         <v>42</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="I6" s="11">
         <v>0.39</v>
@@ -1080,7 +1059,7 @@
         <v>42</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="I7" s="11">
         <v>1.64</v>
@@ -1100,10 +1079,10 @@
         <v>9</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>12</v>
@@ -1115,13 +1094,13 @@
         <v>42</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="I8" s="7">
         <v>2.89</v>
       </c>
       <c r="J8" s="7">
-        <f>I8*F8</f>
+        <f t="shared" ref="J8:J19" si="3">I8*F8</f>
         <v>5.78</v>
       </c>
       <c r="K8" s="9"/>
@@ -1141,7 +1120,7 @@
         <v>40</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F9" s="5">
         <v>3</v>
@@ -1156,12 +1135,12 @@
         <v>0.9</v>
       </c>
       <c r="J9" s="7">
-        <f>I9*F9</f>
+        <f t="shared" si="3"/>
         <v>2.7</v>
       </c>
       <c r="K9" s="9"/>
     </row>
-    <row r="10" spans="1:11" s="2" customFormat="1" ht="28.5">
+    <row r="10" spans="1:11" s="2" customFormat="1" ht="42.75">
       <c r="A10" s="5">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -1176,10 +1155,10 @@
         <v>44</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="F10" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>42</v>
@@ -1191,8 +1170,8 @@
         <v>0.2</v>
       </c>
       <c r="J10" s="7">
-        <f>I10*F10</f>
-        <v>0.60000000000000009</v>
+        <f t="shared" si="3"/>
+        <v>0.8</v>
       </c>
       <c r="K10" s="9"/>
     </row>
@@ -1211,7 +1190,7 @@
         <v>47</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F11" s="5">
         <v>3</v>
@@ -1226,7 +1205,7 @@
         <v>0.18</v>
       </c>
       <c r="J11" s="7">
-        <f>I11*F11</f>
+        <f t="shared" si="3"/>
         <v>0.54</v>
       </c>
       <c r="K11" s="9"/>
@@ -1246,7 +1225,7 @@
         <v>49</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F12" s="5">
         <f>F11*4 + F16*2</f>
@@ -1262,7 +1241,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="J12" s="7">
-        <f>I12*F12</f>
+        <f t="shared" si="3"/>
         <v>2.5200000000000005</v>
       </c>
       <c r="K12" s="9"/>
@@ -1297,7 +1276,7 @@
         <v>0.21</v>
       </c>
       <c r="J13" s="7">
-        <f>I13*F13</f>
+        <f t="shared" si="3"/>
         <v>0.42</v>
       </c>
       <c r="K13" s="9"/>
@@ -1317,7 +1296,7 @@
         <v>61</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F14" s="5">
         <v>3</v>
@@ -1332,12 +1311,12 @@
         <v>0.33</v>
       </c>
       <c r="J14" s="7">
-        <f>I14*F14</f>
+        <f t="shared" si="3"/>
         <v>0.99</v>
       </c>
       <c r="K14" s="9"/>
     </row>
-    <row r="15" spans="1:11" s="2" customFormat="1" ht="28.5">
+    <row r="15" spans="1:11" s="2" customFormat="1" ht="42.75">
       <c r="A15" s="5">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -1352,10 +1331,10 @@
         <v>64</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="F15" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>42</v>
@@ -1367,8 +1346,8 @@
         <v>0.16</v>
       </c>
       <c r="J15" s="7">
-        <f>I15*F15</f>
-        <v>0.48</v>
+        <f t="shared" si="3"/>
+        <v>0.96</v>
       </c>
       <c r="K15" s="9"/>
     </row>
@@ -1387,7 +1366,7 @@
         <v>67</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="F16" s="5">
         <v>3</v>
@@ -1402,64 +1381,63 @@
         <v>0.13</v>
       </c>
       <c r="J16" s="7">
-        <f>I16*F16</f>
+        <f t="shared" si="3"/>
         <v>0.39</v>
       </c>
       <c r="K16" s="9"/>
     </row>
-    <row r="17" spans="1:11" s="2" customFormat="1" ht="28.5">
+    <row r="17" spans="1:10" ht="57">
       <c r="A17" s="5">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="8">
+        <v>1</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="I17" s="13">
+        <v>0.99</v>
+      </c>
+      <c r="J17" s="13">
+        <f t="shared" si="3"/>
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="28.5">
+      <c r="A18" s="5">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F17" s="5">
-        <v>3</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="I17" s="7">
-        <v>0.18</v>
-      </c>
-      <c r="J17" s="7">
-        <f>I17*F17</f>
-        <v>0.54</v>
-      </c>
-      <c r="K17" s="9"/>
-    </row>
-    <row r="18" spans="1:11" s="2" customFormat="1" ht="28.5">
-      <c r="A18" s="5">
-        <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" s="5" t="s">
+      <c r="C18" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="D18" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F18" s="5">
+      <c r="E18" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="8">
         <v>1</v>
       </c>
       <c r="G18" s="5" t="s">
@@ -1468,192 +1446,131 @@
       <c r="H18" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="I18" s="7">
-        <v>0.65</v>
-      </c>
-      <c r="J18" s="7">
-        <f>I18*F18</f>
-        <v>0.65</v>
-      </c>
-      <c r="K18" s="9"/>
-    </row>
-    <row r="19" spans="1:11" ht="57">
+      <c r="I18" s="13">
+        <v>0.45</v>
+      </c>
+      <c r="J18" s="13">
+        <f t="shared" si="3"/>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="28.5">
       <c r="A19" s="5">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="F19" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>42</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="I19" s="13">
-        <v>0.99</v>
+        <v>0.82</v>
       </c>
       <c r="J19" s="13">
-        <f>I19*F19</f>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="28.5">
+        <f t="shared" si="3"/>
+        <v>1.64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="42.75">
       <c r="A20" s="5">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="F20" s="8">
-        <v>1</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="I20" s="13">
-        <v>0.45</v>
-      </c>
-      <c r="J20" s="13">
-        <f>I20*F20</f>
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="28.5">
+      <c r="B20" s="8"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="10">
+        <v>5</v>
+      </c>
+      <c r="G20" s="8"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="7"/>
+    </row>
+    <row r="21" spans="1:10" ht="28.5">
       <c r="A21" s="5">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="F21" s="8">
-        <v>2</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="I21" s="13">
-        <v>0.82</v>
-      </c>
-      <c r="J21" s="13">
-        <f>I21*F21</f>
-        <v>1.64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="42.75">
-      <c r="A22" s="5">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" s="10">
-        <v>5</v>
-      </c>
-      <c r="G22" s="8"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="7"/>
-    </row>
-    <row r="23" spans="1:11" ht="28.5">
-      <c r="A23" s="5">
-        <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="5" t="s">
+      <c r="B21" s="8"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E21" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F21" s="10">
         <v>4</v>
       </c>
-      <c r="G23" s="8"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="7"/>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="G21" s="8"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="7"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:10">
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:10">
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:10">
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:10">
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:10">
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:10">
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:10">
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:10">
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:10">
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
     </row>
@@ -1664,14 +1581,6 @@
     <row r="34" spans="9:10">
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
-    </row>
-    <row r="35" spans="9:10">
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-    </row>
-    <row r="36" spans="9:10">
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1685,19 +1594,17 @@
     <hyperlink ref="H16" r:id="rId8"/>
     <hyperlink ref="H17" r:id="rId9"/>
     <hyperlink ref="H18" r:id="rId10"/>
-    <hyperlink ref="H19" r:id="rId11"/>
-    <hyperlink ref="H20" r:id="rId12"/>
-    <hyperlink ref="H21" r:id="rId13"/>
-    <hyperlink ref="H8" r:id="rId14"/>
-    <hyperlink ref="H7" r:id="rId15"/>
-    <hyperlink ref="H6" r:id="rId16"/>
-    <hyperlink ref="H5" r:id="rId17"/>
-    <hyperlink ref="H4" r:id="rId18"/>
-    <hyperlink ref="H3" r:id="rId19"/>
-    <hyperlink ref="H2" r:id="rId20"/>
+    <hyperlink ref="H8" r:id="rId11"/>
+    <hyperlink ref="H7" r:id="rId12"/>
+    <hyperlink ref="H6" r:id="rId13"/>
+    <hyperlink ref="H5" r:id="rId14"/>
+    <hyperlink ref="H4" r:id="rId15"/>
+    <hyperlink ref="H3" r:id="rId16"/>
+    <hyperlink ref="H2" r:id="rId17"/>
+    <hyperlink ref="H19" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId21"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId19"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updated power entery to baord
</commit_message>
<xml_diff>
--- a/dwg/roboCoolerBOM.xlsx
+++ b/dwg/roboCoolerBOM.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="110">
   <si>
     <t>Item</t>
   </si>
@@ -315,6 +315,42 @@
   </si>
   <si>
     <t>D2 D3 D4 D5 D6</t>
+  </si>
+  <si>
+    <t>J6 J7</t>
+  </si>
+  <si>
+    <t>Barrel Jack</t>
+  </si>
+  <si>
+    <t>Barrel Plug</t>
+  </si>
+  <si>
+    <t>J8</t>
+  </si>
+  <si>
+    <t>USB Mini Connector</t>
+  </si>
+  <si>
+    <t>100uF Capacitors</t>
+  </si>
+  <si>
+    <t>C16-C19</t>
+  </si>
+  <si>
+    <t>Fuse Holder</t>
+  </si>
+  <si>
+    <t>F1 F2</t>
+  </si>
+  <si>
+    <t>4A Fuse</t>
+  </si>
+  <si>
+    <t>12V PSU</t>
+  </si>
+  <si>
+    <t>5V PSU</t>
   </si>
 </sst>
 </file>
@@ -382,12 +418,18 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -477,7 +519,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -518,6 +560,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -825,9 +882,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -835,7 +894,7 @@
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.28515625" customWidth="1"/>
     <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
@@ -876,7 +935,7 @@
         <v>10</v>
       </c>
       <c r="K1" s="12">
-        <f>SUM(J2:J99)</f>
+        <f>SUM(J2:J101)</f>
         <v>29.580000000000002</v>
       </c>
     </row>
@@ -916,7 +975,7 @@
     </row>
     <row r="3" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <f t="shared" ref="A3:A22" si="1">A2+1</f>
+        <f t="shared" ref="A3:A30" si="1">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -1585,36 +1644,168 @@
       <c r="J22" s="7"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
+      <c r="A23" s="18">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="18"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="F23" s="19">
+        <v>2</v>
+      </c>
+      <c r="G23" s="18"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="22"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
+      <c r="A24" s="18">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="18"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="F24" s="19">
+        <v>2</v>
+      </c>
+      <c r="G24" s="18"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="22"/>
+    </row>
+    <row r="25" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="18">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="18"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="F25" s="19">
+        <v>4</v>
+      </c>
+      <c r="G25" s="18"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="22"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
+      <c r="A26" s="18">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="18"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="F26" s="19">
+        <v>1</v>
+      </c>
+      <c r="G26" s="18"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="22"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
+      <c r="A27" s="18">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="18"/>
+      <c r="C27" s="19">
+        <v>3568</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="F27" s="19">
+        <v>2</v>
+      </c>
+      <c r="G27" s="18"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="22"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
+      <c r="A28" s="18">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="18"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19">
+        <v>2</v>
+      </c>
+      <c r="G28" s="18"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="22"/>
+    </row>
+    <row r="29" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="18">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="18"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19">
+        <v>1</v>
+      </c>
+      <c r="G29" s="18"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="22"/>
+    </row>
+    <row r="30" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="18">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="18"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19">
+        <v>1</v>
+      </c>
+      <c r="G30" s="18"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="22"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I31" s="4"/>
@@ -1635,6 +1826,14 @@
     <row r="35" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
+    </row>
+    <row r="36" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+    </row>
+    <row r="37" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
removed erc errors from schematic
</commit_message>
<xml_diff>
--- a/dwg/roboCoolerBOM.xlsx
+++ b/dwg/roboCoolerBOM.xlsx
@@ -329,9 +329,6 @@
     <t>J8</t>
   </si>
   <si>
-    <t>USB Mini Connector</t>
-  </si>
-  <si>
     <t>100uF Capacitors</t>
   </si>
   <si>
@@ -351,6 +348,9 @@
   </si>
   <si>
     <t>5V PSU</t>
+  </si>
+  <si>
+    <t>USB Connector</t>
   </si>
 </sst>
 </file>
@@ -884,8 +884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1693,10 +1693,10 @@
       <c r="B25" s="18"/>
       <c r="C25" s="19"/>
       <c r="D25" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="E25" s="19" t="s">
         <v>103</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>104</v>
       </c>
       <c r="F25" s="19">
         <v>4</v>
@@ -1714,7 +1714,7 @@
       <c r="B26" s="18"/>
       <c r="C26" s="19"/>
       <c r="D26" s="18" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E26" s="19" t="s">
         <v>101</v>
@@ -1737,10 +1737,10 @@
         <v>3568</v>
       </c>
       <c r="D27" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="E27" s="19" t="s">
         <v>105</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>106</v>
       </c>
       <c r="F27" s="19">
         <v>2</v>
@@ -1758,7 +1758,7 @@
       <c r="B28" s="18"/>
       <c r="C28" s="19"/>
       <c r="D28" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E28" s="19"/>
       <c r="F28" s="19">
@@ -1777,7 +1777,7 @@
       <c r="B29" s="18"/>
       <c r="C29" s="19"/>
       <c r="D29" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E29" s="19"/>
       <c r="F29" s="19">
@@ -1796,7 +1796,7 @@
       <c r="B30" s="18"/>
       <c r="C30" s="19"/>
       <c r="D30" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E30" s="19"/>
       <c r="F30" s="19">

</xml_diff>

<commit_message>
updated conn for capsense out and hal sensors
</commit_message>
<xml_diff>
--- a/dwg/roboCoolerBOM.xlsx
+++ b/dwg/roboCoolerBOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="124">
   <si>
     <t>Item</t>
   </si>
@@ -240,9 +240,6 @@
     <t>S7045-ND</t>
   </si>
   <si>
-    <t>J7</t>
-  </si>
-  <si>
     <t>TDK</t>
   </si>
   <si>
@@ -367,6 +364,33 @@
   </si>
   <si>
     <t>IC MOTOR DRIVER PAR 20HSOP</t>
+  </si>
+  <si>
+    <t>J7 J13 J14</t>
+  </si>
+  <si>
+    <t>Molex</t>
+  </si>
+  <si>
+    <t>WM8275-ND</t>
+  </si>
+  <si>
+    <t>6 Positions Header, Shrouded Connector 0.100" (2.54mm) Through Hole, Right Angle Gold</t>
+  </si>
+  <si>
+    <t>WM8035-ND</t>
+  </si>
+  <si>
+    <t>CONN HOUSING 6POS .100" DUAL</t>
+  </si>
+  <si>
+    <t>P7 P13 P14</t>
+  </si>
+  <si>
+    <t>Socket Contact Gold 22-24 AWG Crimp</t>
+  </si>
+  <si>
+    <t>WM2580CT-ND</t>
   </si>
 </sst>
 </file>
@@ -406,38 +430,38 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-      <scheme val="major"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-      <scheme val="major"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-      <scheme val="major"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -638,126 +662,90 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1064,321 +1052,321 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="10" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="10"/>
+    <col min="1" max="1" width="6.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="2">
-        <f>SUM(J2:J70)</f>
-        <v>27.439999999999998</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="6" customFormat="1" ht="71.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="21">
+      <c r="K1" s="10">
+        <f>SUM(J2:J72)</f>
+        <v>37.340000000000003</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2" s="13">
         <v>4</v>
       </c>
-      <c r="G2" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="36" t="s">
+      <c r="G2" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="I2" s="25">
+      <c r="I2" s="14">
         <v>0.12</v>
       </c>
-      <c r="J2" s="26">
-        <f>I2*F2</f>
+      <c r="J2" s="15">
+        <f t="shared" ref="J2:J7" si="0">I2*F2</f>
         <v>0.48</v>
       </c>
-      <c r="K2" s="14"/>
-    </row>
-    <row r="3" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="27">
+      <c r="K2" s="5"/>
+    </row>
+    <row r="3" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" s="19" t="s">
+      <c r="B3" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="D3" s="38" t="s">
-        <v>79</v>
-      </c>
       <c r="E3" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F3" s="7">
         <v>5</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="38" t="s">
+      <c r="G3" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0.11</v>
+      </c>
+      <c r="J3" s="18">
+        <f t="shared" si="0"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
+        <f t="shared" ref="A4:A29" si="1">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="I3" s="37">
-        <v>0.11</v>
-      </c>
-      <c r="J3" s="28">
-        <f>I3*F3</f>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="K3" s="39"/>
-    </row>
-    <row r="4" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A4" s="27">
-        <f t="shared" ref="A4:A27" si="0">A3+1</f>
-        <v>3</v>
-      </c>
-      <c r="B4" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" s="19" t="s">
+      <c r="D4" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="38" t="s">
-        <v>82</v>
-      </c>
       <c r="E4" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F4" s="7">
         <v>2</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="38" t="s">
+      <c r="G4" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="I4" s="7">
+        <v>0.18</v>
+      </c>
+      <c r="J4" s="18">
+        <f t="shared" si="0"/>
+        <v>0.36</v>
+      </c>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="16">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="I4" s="37">
-        <v>0.18</v>
-      </c>
-      <c r="J4" s="28">
-        <f>I4*F4</f>
-        <v>0.36</v>
-      </c>
-      <c r="K4" s="39"/>
-    </row>
-    <row r="5" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="27">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B5" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" s="19" t="s">
+      <c r="D5" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="D5" s="38" t="s">
-        <v>85</v>
-      </c>
       <c r="E5" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F5" s="7">
         <v>4</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="I5" s="37">
+      <c r="G5" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="I5" s="7">
         <v>0.14000000000000001</v>
       </c>
-      <c r="J5" s="28">
-        <f>I5*F5</f>
+      <c r="J5" s="18">
+        <f t="shared" si="0"/>
         <v>0.56000000000000005</v>
       </c>
-      <c r="K5" s="39"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="27">
-        <f t="shared" si="0"/>
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="16">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="D6" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="D6" s="38" t="s">
-        <v>76</v>
-      </c>
       <c r="E6" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F6" s="7">
         <v>3</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="I6" s="37">
+      <c r="G6" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="I6" s="7">
         <v>0.14000000000000001</v>
       </c>
-      <c r="J6" s="28">
-        <f>I6*F6</f>
+      <c r="J6" s="18">
+        <f t="shared" si="0"/>
         <v>0.42000000000000004</v>
       </c>
-      <c r="K6" s="39"/>
-    </row>
-    <row r="7" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A7" s="27">
-        <f t="shared" si="0"/>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="16">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B7" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" s="19" t="s">
+      <c r="B7" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="38" t="s">
-        <v>88</v>
-      </c>
       <c r="E7" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F7" s="7">
         <v>1</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="38" t="s">
-        <v>89</v>
-      </c>
-      <c r="I7" s="37">
+      <c r="G7" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="I7" s="7">
         <v>0.35</v>
       </c>
-      <c r="J7" s="28">
-        <f>I7*F7</f>
+      <c r="J7" s="18">
+        <f t="shared" si="0"/>
         <v>0.35</v>
       </c>
-      <c r="K7" s="39"/>
-    </row>
-    <row r="8" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="27">
-        <f t="shared" si="0"/>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="17" t="s">
         <v>33</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="17" t="s">
         <v>34</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F8" s="7">
         <v>2</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="4" t="s">
+      <c r="G8" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="20">
         <v>0.4</v>
       </c>
-      <c r="J8" s="29">
-        <f t="shared" ref="J8" si="1">I8*F8</f>
+      <c r="J8" s="21">
+        <f t="shared" ref="J8" si="2">I8*F8</f>
         <v>0.8</v>
       </c>
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="27">
-        <f t="shared" si="0"/>
+      <c r="A9" s="16">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="17" t="s">
         <v>52</v>
       </c>
       <c r="C9" s="7">
         <v>3568</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="17" t="s">
         <v>36</v>
       </c>
       <c r="E9" s="7" t="s">
@@ -1387,33 +1375,33 @@
       <c r="F9" s="7">
         <v>2</v>
       </c>
-      <c r="G9" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="38" t="s">
+      <c r="G9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="20">
         <v>0.98</v>
       </c>
-      <c r="J9" s="28">
+      <c r="J9" s="18">
         <f>I9*F9</f>
         <v>1.96</v>
       </c>
-      <c r="K9" s="13"/>
+      <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="27">
-        <f t="shared" si="0"/>
+      <c r="A10" s="16">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="7" t="s">
         <v>56</v>
       </c>
       <c r="E10" s="7" t="s">
@@ -1422,138 +1410,138 @@
       <c r="F10" s="7">
         <v>2</v>
       </c>
-      <c r="G10" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="37" t="s">
+      <c r="G10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="20">
         <v>0.47</v>
       </c>
-      <c r="J10" s="28">
+      <c r="J10" s="18">
         <f>I10*F10</f>
         <v>0.94</v>
       </c>
-      <c r="K10" s="39"/>
-    </row>
-    <row r="11" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="27">
-        <f t="shared" si="0"/>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="16">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="7" t="s">
         <v>43</v>
       </c>
       <c r="F11" s="7">
         <v>2</v>
       </c>
-      <c r="G11" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="19" t="s">
+      <c r="G11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="20">
         <v>1.34</v>
       </c>
-      <c r="J11" s="28">
-        <f t="shared" ref="J11" si="2">I11*F11</f>
+      <c r="J11" s="18">
+        <f t="shared" ref="J11" si="3">I11*F11</f>
         <v>2.68</v>
       </c>
-      <c r="K11" s="13"/>
+      <c r="K11" s="5"/>
     </row>
     <row r="12" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="27">
-        <f t="shared" si="0"/>
+      <c r="A12" s="16">
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="7" t="s">
         <v>43</v>
       </c>
       <c r="F12" s="7">
         <v>2</v>
       </c>
-      <c r="G12" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" s="38" t="s">
+      <c r="G12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="20">
         <v>0.55000000000000004</v>
       </c>
-      <c r="J12" s="28">
+      <c r="J12" s="18">
         <f>I12*F12</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="K12" s="13"/>
-    </row>
-    <row r="13" spans="1:11" s="11" customFormat="1" ht="57" x14ac:dyDescent="0.25">
-      <c r="A13" s="27">
-        <f t="shared" si="0"/>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="16">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="17">
         <v>2</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="4" t="s">
+      <c r="G13" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="I13" s="9">
+      <c r="I13" s="22">
         <v>2.89</v>
       </c>
-      <c r="J13" s="29">
+      <c r="J13" s="21">
         <f>I13*F13</f>
         <v>5.78</v>
       </c>
       <c r="K13" s="5"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="27">
-        <f t="shared" si="0"/>
+    <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="16">
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="38" t="s">
+      <c r="D14" s="29" t="s">
         <v>66</v>
       </c>
       <c r="E14" s="7" t="s">
@@ -1562,33 +1550,33 @@
       <c r="F14" s="7">
         <v>1</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="19" t="s">
+      <c r="G14" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="I14" s="37">
+      <c r="I14" s="7">
         <v>0.7</v>
       </c>
-      <c r="J14" s="28">
+      <c r="J14" s="18">
         <f>I14*F14</f>
         <v>0.7</v>
       </c>
-      <c r="K14" s="39"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="27">
-        <f t="shared" si="0"/>
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="16">
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="38" t="s">
+      <c r="D15" s="29" t="s">
         <v>70</v>
       </c>
       <c r="E15" s="7" t="s">
@@ -1597,397 +1585,483 @@
       <c r="F15" s="7">
         <v>1</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" s="38" t="s">
+      <c r="G15" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="I15" s="37">
+      <c r="I15" s="7">
         <v>1.01</v>
       </c>
-      <c r="J15" s="28">
+      <c r="J15" s="18">
         <f>I15*F15</f>
         <v>1.01</v>
       </c>
-      <c r="K15" s="39"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="27">
-        <f t="shared" si="0"/>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="16">
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="38" t="s">
-        <v>70</v>
+      <c r="B16" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16" s="29">
+        <v>901303206</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>118</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>73</v>
+        <v>115</v>
       </c>
       <c r="F16" s="7">
-        <v>1</v>
-      </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="39"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="27">
-        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="I16" s="7">
+        <v>1.55</v>
+      </c>
+      <c r="J16" s="18">
+        <f>I16*F16</f>
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="16">
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="38" t="s">
-        <v>104</v>
+      <c r="B17" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="29">
+        <v>901420006</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>120</v>
       </c>
       <c r="E17" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F17" s="7">
+        <f>F16</f>
+        <v>3</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="I17" s="7">
+        <v>0.43</v>
+      </c>
+      <c r="J17" s="18">
+        <f>I17*F17</f>
+        <v>1.29</v>
+      </c>
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="16">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C18" s="29">
+        <v>901190110</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F18" s="7">
+        <f>F17*6</f>
+        <v>18</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="I18" s="7">
+        <v>0.22</v>
+      </c>
+      <c r="J18" s="18">
+        <f>I18*F18</f>
+        <v>3.96</v>
+      </c>
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="16">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29" t="s">
         <v>103</v>
-      </c>
-      <c r="F17" s="7">
-        <v>2</v>
-      </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="39"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="27">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B18" s="37"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="38" t="s">
-        <v>105</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="F18" s="7">
-        <v>2</v>
-      </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="39"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="27">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>102</v>
       </c>
       <c r="F19" s="7">
-        <v>1</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="I19" s="8">
-        <v>0.63</v>
-      </c>
-      <c r="J19" s="28">
-        <f t="shared" ref="J19" si="3">I19*F19</f>
-        <v>0.63</v>
-      </c>
-      <c r="K19" s="13"/>
+        <v>2</v>
+      </c>
+      <c r="G19" s="17"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="5"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="27">
-        <f t="shared" si="0"/>
+      <c r="A20" s="16">
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="1" t="s">
-        <v>101</v>
+      <c r="B20" s="7"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29" t="s">
+        <v>104</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F20" s="7">
         <v>2</v>
       </c>
-      <c r="G20" s="18"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="13"/>
-    </row>
-    <row r="21" spans="1:11" s="11" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="27">
-        <f t="shared" si="0"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="16">
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H21" s="4" t="s">
+      <c r="B21" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F21" s="7">
+        <v>1</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="I21" s="20">
+        <v>0.63</v>
+      </c>
+      <c r="J21" s="18">
+        <f t="shared" ref="J21" si="4">I21*F21</f>
+        <v>0.63</v>
+      </c>
+      <c r="K21" s="5"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="16">
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="I21" s="9">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="J21" s="29">
-        <f>I21*F21</f>
-        <v>0</v>
-      </c>
-      <c r="K21" s="5"/>
-    </row>
-    <row r="22" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="27">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B22" s="37" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="37" t="s">
-        <v>63</v>
+      <c r="B22" s="17"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="17" t="s">
+        <v>100</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>99</v>
       </c>
       <c r="F22" s="7">
+        <v>2</v>
+      </c>
+      <c r="G22" s="7"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="16">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23" s="22">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J23" s="21">
+        <f>I23*F23</f>
+        <v>0</v>
+      </c>
+      <c r="K23" s="5"/>
+    </row>
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="16">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F24" s="7">
         <v>8</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H22" s="38" t="s">
+      <c r="G24" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="I22" s="12">
+      <c r="I24" s="20">
         <v>0.1</v>
       </c>
-      <c r="J22" s="28">
-        <f>I22*F22</f>
+      <c r="J24" s="18">
+        <f>I24*F24</f>
         <v>0.8</v>
       </c>
-      <c r="K22" s="39"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="27">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B23" s="37" t="s">
+      <c r="K24" s="5"/>
+    </row>
+    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="16">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="37" t="s">
+      <c r="C25" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="D23" s="38" t="s">
+      <c r="E25" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F25" s="7">
+        <v>3</v>
+      </c>
+      <c r="G25" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="F23" s="7">
-        <v>3</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="I23" s="12">
+      <c r="I25" s="20">
         <v>0.1</v>
       </c>
-      <c r="J23" s="28">
-        <f>I23*F23</f>
+      <c r="J25" s="18">
+        <f>I25*F25</f>
         <v>0.30000000000000004</v>
       </c>
-      <c r="K23" s="13"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="27">
-        <f t="shared" si="0"/>
+      <c r="K25" s="5"/>
+    </row>
+    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="16">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F26" s="7">
+        <v>2</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="I26" s="20">
+        <v>0.78</v>
+      </c>
+      <c r="J26" s="18">
+        <f>I26*F26</f>
+        <v>1.56</v>
+      </c>
+      <c r="K26" s="5"/>
+    </row>
+    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="16">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="40" t="s">
-        <v>108</v>
-      </c>
-      <c r="D24" s="41" t="s">
-        <v>109</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="F24" s="7">
+      <c r="C27" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" s="17">
         <v>2</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H24" s="41" t="s">
+      <c r="G27" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H27" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="I27" s="20">
+        <v>0.82</v>
+      </c>
+      <c r="J27" s="18">
+        <f>I27*F27</f>
+        <v>1.64</v>
+      </c>
+      <c r="K27" s="5"/>
+    </row>
+    <row r="28" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="16">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="17">
+        <v>1</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H28" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="I28" s="22">
+        <v>0.49</v>
+      </c>
+      <c r="J28" s="21">
+        <f t="shared" ref="J28" si="5">I28*F28</f>
+        <v>0.49</v>
+      </c>
+      <c r="K28" s="5"/>
+    </row>
+    <row r="29" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="23">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="I24" s="12">
-        <v>0.78</v>
-      </c>
-      <c r="J24" s="28">
-        <f>I24*F24</f>
-        <v>1.56</v>
-      </c>
-      <c r="K24" s="13"/>
-    </row>
-    <row r="25" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="27">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" s="1">
-        <v>2</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I25" s="12">
-        <v>0.82</v>
-      </c>
-      <c r="J25" s="28">
-        <f>I25*F25</f>
-        <v>1.64</v>
-      </c>
-      <c r="K25" s="13"/>
-    </row>
-    <row r="26" spans="1:11" s="6" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="27">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="1">
+      <c r="D29" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="24">
         <v>1</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I26" s="9">
-        <v>0.49</v>
-      </c>
-      <c r="J26" s="29">
-        <f t="shared" ref="J26" si="4">I26*F26</f>
-        <v>0.49</v>
-      </c>
-      <c r="K26" s="5"/>
-    </row>
-    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="30">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B27" s="42" t="s">
+      <c r="G29" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H29" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="C27" s="42" t="s">
-        <v>112</v>
-      </c>
-      <c r="D27" s="43" t="s">
-        <v>115</v>
-      </c>
-      <c r="E27" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" s="31">
-        <v>1</v>
-      </c>
-      <c r="G27" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="H27" s="43" t="s">
-        <v>114</v>
-      </c>
-      <c r="I27" s="33">
+      <c r="I29" s="26">
         <v>4.33</v>
       </c>
-      <c r="J27" s="34">
-        <f t="shared" ref="J27" si="5">I27*F27</f>
+      <c r="J29" s="27">
+        <f t="shared" ref="J29" si="6">I29*F29</f>
         <v>4.33</v>
       </c>
-      <c r="K27" s="39"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G29" s="15"/>
+      <c r="K29" s="5"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G31" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H21" r:id="rId1"/>
+    <hyperlink ref="H23" r:id="rId1"/>
     <hyperlink ref="H13" r:id="rId2"/>
-    <hyperlink ref="H26" r:id="rId3"/>
-    <hyperlink ref="H25" r:id="rId4"/>
+    <hyperlink ref="H28" r:id="rId3"/>
+    <hyperlink ref="H27" r:id="rId4"/>
     <hyperlink ref="H8" r:id="rId5" display="BAT42CT-ND"/>
+    <hyperlink ref="H16" r:id="rId6" display=" WM8275-ND"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
moved led fan and pump to 6-pin conns
</commit_message>
<xml_diff>
--- a/dwg/roboCoolerBOM.xlsx
+++ b/dwg/roboCoolerBOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="118">
   <si>
     <t>Item</t>
   </si>
@@ -288,21 +288,12 @@
     <t>445-5984-1-ND</t>
   </si>
   <si>
-    <t>C8 C12</t>
-  </si>
-  <si>
-    <t>C9-C11 C19</t>
-  </si>
-  <si>
     <t>C13-C15</t>
   </si>
   <si>
     <t>C16</t>
   </si>
   <si>
-    <t>C5-C7 C17 C18</t>
-  </si>
-  <si>
     <t>ERJ-6ENF1001V</t>
   </si>
   <si>
@@ -318,27 +309,9 @@
     <t>R1-R4 R8-R11</t>
   </si>
   <si>
-    <t>J13 J14</t>
-  </si>
-  <si>
-    <t>3 Pin Connector</t>
-  </si>
-  <si>
     <t>J12</t>
   </si>
   <si>
-    <t>J8 J9</t>
-  </si>
-  <si>
-    <t>2 Pin Connector</t>
-  </si>
-  <si>
-    <t>4 Pin Connector</t>
-  </si>
-  <si>
-    <t>J10 J11</t>
-  </si>
-  <si>
     <t>D1 D2</t>
   </si>
   <si>
@@ -366,9 +339,6 @@
     <t>IC MOTOR DRIVER PAR 20HSOP</t>
   </si>
   <si>
-    <t>J7 J13 J14</t>
-  </si>
-  <si>
     <t>Molex</t>
   </si>
   <si>
@@ -384,13 +354,25 @@
     <t>CONN HOUSING 6POS .100" DUAL</t>
   </si>
   <si>
-    <t>P7 P13 P14</t>
-  </si>
-  <si>
     <t>Socket Contact Gold 22-24 AWG Crimp</t>
   </si>
   <si>
     <t>WM2580CT-ND</t>
+  </si>
+  <si>
+    <t>C5 C6 C17 C18</t>
+  </si>
+  <si>
+    <t>C9 C10 C19</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>J7 J8 J10 J13 J14</t>
+  </si>
+  <si>
+    <t>P7 P8 P10 P13 P14</t>
   </si>
 </sst>
 </file>
@@ -1052,11 +1034,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,8 +1089,8 @@
         <v>10</v>
       </c>
       <c r="K1" s="10">
-        <f>SUM(J2:J72)</f>
-        <v>37.340000000000003</v>
+        <f>SUM(J2:J69)</f>
+        <v>43.51</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -1160,10 +1142,10 @@
         <v>78</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="F3" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G3" s="17" t="s">
         <v>18</v>
@@ -1176,13 +1158,13 @@
       </c>
       <c r="J3" s="18">
         <f t="shared" si="0"/>
-        <v>0.55000000000000004</v>
+        <v>0.44</v>
       </c>
       <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
-        <f t="shared" ref="A4:A29" si="1">A3+1</f>
+        <f t="shared" ref="A4:A26" si="1">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
@@ -1195,10 +1177,10 @@
         <v>81</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="F4" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" s="17" t="s">
         <v>18</v>
@@ -1211,7 +1193,7 @@
       </c>
       <c r="J4" s="18">
         <f t="shared" si="0"/>
-        <v>0.36</v>
+        <v>0.18</v>
       </c>
       <c r="K4" s="5"/>
     </row>
@@ -1230,10 +1212,10 @@
         <v>84</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="F5" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5" s="17" t="s">
         <v>18</v>
@@ -1246,7 +1228,7 @@
       </c>
       <c r="J5" s="18">
         <f t="shared" si="0"/>
-        <v>0.56000000000000005</v>
+        <v>0.42000000000000004</v>
       </c>
       <c r="K5" s="5"/>
     </row>
@@ -1265,7 +1247,7 @@
         <v>75</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F6" s="7">
         <v>3</v>
@@ -1300,7 +1282,7 @@
         <v>87</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F7" s="7">
         <v>1</v>
@@ -1335,7 +1317,7 @@
         <v>34</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="F8" s="7">
         <v>2</v>
@@ -1490,7 +1472,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="J12" s="18">
-        <f>I12*F12</f>
+        <f t="shared" ref="J12:J18" si="4">I12*F12</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="K12" s="5"/>
@@ -1525,7 +1507,7 @@
         <v>2.89</v>
       </c>
       <c r="J13" s="21">
-        <f>I13*F13</f>
+        <f t="shared" si="4"/>
         <v>5.78</v>
       </c>
       <c r="K13" s="5"/>
@@ -1560,7 +1542,7 @@
         <v>0.7</v>
       </c>
       <c r="J14" s="18">
-        <f>I14*F14</f>
+        <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
       <c r="K14" s="5"/>
@@ -1595,7 +1577,7 @@
         <v>1.01</v>
       </c>
       <c r="J15" s="18">
-        <f>I15*F15</f>
+        <f t="shared" si="4"/>
         <v>1.01</v>
       </c>
       <c r="K15" s="5"/>
@@ -1606,104 +1588,105 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C16" s="29">
         <v>901303206</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F16" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G16" s="17" t="s">
         <v>18</v>
       </c>
       <c r="H16" s="19" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="I16" s="7">
         <v>1.55</v>
       </c>
       <c r="J16" s="18">
-        <f>I16*F16</f>
-        <v>4.6500000000000004</v>
+        <f t="shared" si="4"/>
+        <v>7.75</v>
       </c>
       <c r="K16" s="5"/>
     </row>
-    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C17" s="29">
         <v>901420006</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F17" s="7">
         <f>F16</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G17" s="17" t="s">
         <v>18</v>
       </c>
       <c r="H17" s="19" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="I17" s="7">
         <v>0.43</v>
       </c>
       <c r="J17" s="18">
-        <f>I17*F17</f>
-        <v>1.29</v>
+        <f t="shared" si="4"/>
+        <v>2.15</v>
       </c>
       <c r="K17" s="5"/>
     </row>
-    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="16">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C18" s="29">
         <v>901190110</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>121</v>
+        <v>111</v>
+      </c>
+      <c r="E18" s="7" t="str">
+        <f>E17</f>
+        <v>P7 P8 P10 P13 P14</v>
       </c>
       <c r="F18" s="7">
         <f>F17*6</f>
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="G18" s="17" t="s">
         <v>18</v>
       </c>
       <c r="H18" s="19" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="I18" s="7">
         <v>0.22</v>
       </c>
       <c r="J18" s="18">
-        <f>I18*F18</f>
-        <v>3.96</v>
+        <f t="shared" si="4"/>
+        <v>6.6</v>
       </c>
       <c r="K18" s="5"/>
     </row>
@@ -1712,130 +1695,169 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29" t="s">
-        <v>103</v>
+      <c r="B19" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>38</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F19" s="7">
+        <v>1</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="I19" s="20">
+        <v>0.63</v>
+      </c>
+      <c r="J19" s="18">
+        <f t="shared" ref="J19" si="5">I19*F19</f>
+        <v>0.63</v>
+      </c>
+      <c r="K19" s="5"/>
+    </row>
+    <row r="20" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="16">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="22">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J20" s="21">
+        <f>I20*F20</f>
+        <v>0</v>
+      </c>
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="16">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F21" s="7">
+        <v>8</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="I21" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="J21" s="18">
+        <f>I21*F21</f>
+        <v>0.8</v>
+      </c>
+      <c r="K21" s="5"/>
+    </row>
+    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="16">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22" s="7">
+        <v>3</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="I22" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="J22" s="18">
+        <f>I22*F22</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="16">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F23" s="7">
         <v>2</v>
       </c>
-      <c r="G19" s="17"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="5"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="16">
-        <f t="shared" si="1"/>
-        <v>19</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="F20" s="7">
-        <v>2</v>
-      </c>
-      <c r="G20" s="17"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="5"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="16">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="7" t="s">
+      <c r="G23" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="F21" s="7">
-        <v>1</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H21" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="I21" s="20">
-        <v>0.63</v>
-      </c>
-      <c r="J21" s="18">
-        <f t="shared" ref="J21" si="4">I21*F21</f>
-        <v>0.63</v>
-      </c>
-      <c r="K21" s="5"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="16">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="F22" s="7">
-        <v>2</v>
-      </c>
-      <c r="G22" s="7"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="5"/>
-    </row>
-    <row r="23" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="16">
-        <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="I23" s="22">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="J23" s="21">
+      <c r="I23" s="20">
+        <v>0.78</v>
+      </c>
+      <c r="J23" s="18">
         <f>I23*F23</f>
-        <v>0</v>
+        <v>1.56</v>
       </c>
       <c r="K23" s="5"/>
     </row>
@@ -1844,220 +1866,115 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="F24" s="7">
-        <v>8</v>
+      <c r="B24" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="17">
+        <v>2</v>
       </c>
       <c r="G24" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="H24" s="29" t="s">
-        <v>64</v>
+      <c r="H24" s="19" t="s">
+        <v>31</v>
       </c>
       <c r="I24" s="20">
-        <v>0.1</v>
+        <v>0.82</v>
       </c>
       <c r="J24" s="18">
         <f>I24*F24</f>
-        <v>0.8</v>
+        <v>1.64</v>
       </c>
       <c r="K24" s="5"/>
     </row>
-    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D25" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="F25" s="7">
-        <v>3</v>
+      <c r="B25" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="17">
+        <v>1</v>
       </c>
       <c r="G25" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="H25" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="I25" s="20">
-        <v>0.1</v>
-      </c>
-      <c r="J25" s="18">
-        <f>I25*F25</f>
-        <v>0.30000000000000004</v>
+      <c r="H25" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="I25" s="22">
+        <v>0.49</v>
+      </c>
+      <c r="J25" s="21">
+        <f t="shared" ref="J25" si="6">I25*F25</f>
+        <v>0.49</v>
       </c>
       <c r="K25" s="5"/>
     </row>
-    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="16">
+    <row r="26" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="23">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="D26" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F26" s="7">
-        <v>2</v>
-      </c>
-      <c r="G26" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="H26" s="30" t="s">
-        <v>110</v>
-      </c>
-      <c r="I26" s="20">
-        <v>0.78</v>
-      </c>
-      <c r="J26" s="18">
-        <f>I26*F26</f>
-        <v>1.56</v>
+      <c r="B26" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="24">
+        <v>1</v>
+      </c>
+      <c r="G26" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="I26" s="26">
+        <v>4.33</v>
+      </c>
+      <c r="J26" s="27">
+        <f t="shared" ref="J26" si="7">I26*F26</f>
+        <v>4.33</v>
       </c>
       <c r="K26" s="5"/>
     </row>
-    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="16">
-        <f t="shared" si="1"/>
-        <v>26</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="F27" s="17">
-        <v>2</v>
-      </c>
-      <c r="G27" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="H27" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="I27" s="20">
-        <v>0.82</v>
-      </c>
-      <c r="J27" s="18">
-        <f>I27*F27</f>
-        <v>1.64</v>
-      </c>
-      <c r="K27" s="5"/>
-    </row>
-    <row r="28" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="16">
-        <f t="shared" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" s="17">
-        <v>1</v>
-      </c>
-      <c r="G28" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="H28" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="I28" s="22">
-        <v>0.49</v>
-      </c>
-      <c r="J28" s="21">
-        <f t="shared" ref="J28" si="5">I28*F28</f>
-        <v>0.49</v>
-      </c>
-      <c r="K28" s="5"/>
-    </row>
-    <row r="29" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="23">
-        <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="B29" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="C29" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="D29" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="E29" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="F29" s="24">
-        <v>1</v>
-      </c>
-      <c r="G29" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="H29" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="I29" s="26">
-        <v>4.33</v>
-      </c>
-      <c r="J29" s="27">
-        <f t="shared" ref="J29" si="6">I29*F29</f>
-        <v>4.33</v>
-      </c>
-      <c r="K29" s="5"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G31" s="6"/>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G28" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H23" r:id="rId1"/>
+    <hyperlink ref="H20" r:id="rId1"/>
     <hyperlink ref="H13" r:id="rId2"/>
-    <hyperlink ref="H28" r:id="rId3"/>
-    <hyperlink ref="H27" r:id="rId4"/>
+    <hyperlink ref="H25" r:id="rId3"/>
+    <hyperlink ref="H24" r:id="rId4"/>
     <hyperlink ref="H8" r:id="rId5" display="BAT42CT-ND"/>
     <hyperlink ref="H16" r:id="rId6" display=" WM8275-ND"/>
   </hyperlinks>

</xml_diff>

<commit_message>
moved J11 to the same 6pin connector.
</commit_message>
<xml_diff>
--- a/dwg/roboCoolerBOM.xlsx
+++ b/dwg/roboCoolerBOM.xlsx
@@ -351,13 +351,13 @@
     <t>C8</t>
   </si>
   <si>
-    <t>J7 J8 J10 J13 J14</t>
-  </si>
-  <si>
-    <t>P7 P8 P10 P13 P14</t>
-  </si>
-  <si>
     <t>R1 R2 R8-R11</t>
+  </si>
+  <si>
+    <t>J7 J8 J10 J11 J13 J14</t>
+  </si>
+  <si>
+    <t>P7 P8 P10 P11 P13 P14</t>
   </si>
 </sst>
 </file>
@@ -1021,9 +1021,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,7 +1075,7 @@
       </c>
       <c r="K1" s="10">
         <f>SUM(J2:J68)</f>
-        <v>41.67</v>
+        <v>44.970000000000006</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -1582,10 +1582,10 @@
         <v>102</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F16" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G16" s="17" t="s">
         <v>18</v>
@@ -1598,7 +1598,7 @@
       </c>
       <c r="J16" s="18">
         <f t="shared" si="4"/>
-        <v>7.75</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="K16" s="5"/>
     </row>
@@ -1617,11 +1617,11 @@
         <v>104</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F17" s="7">
         <f>F16</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G17" s="17" t="s">
         <v>18</v>
@@ -1634,7 +1634,7 @@
       </c>
       <c r="J17" s="18">
         <f t="shared" si="4"/>
-        <v>2.15</v>
+        <v>2.58</v>
       </c>
       <c r="K17" s="5"/>
     </row>
@@ -1654,11 +1654,11 @@
       </c>
       <c r="E18" s="7" t="str">
         <f>E17</f>
-        <v>P7 P8 P10 P13 P14</v>
+        <v>P7 P8 P10 P11 P13 P14</v>
       </c>
       <c r="F18" s="7">
         <f>F17*6</f>
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="G18" s="17" t="s">
         <v>18</v>
@@ -1671,7 +1671,7 @@
       </c>
       <c r="J18" s="18">
         <f t="shared" si="4"/>
-        <v>6.6</v>
+        <v>7.92</v>
       </c>
       <c r="K18" s="5"/>
     </row>
@@ -1756,7 +1756,7 @@
         <v>58</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F21" s="7">
         <v>6</v>

</xml_diff>

<commit_message>
removed unused crimp contacts
</commit_message>
<xml_diff>
--- a/dwg/roboCoolerBOM.xlsx
+++ b/dwg/roboCoolerBOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="109">
   <si>
     <t>Item</t>
   </si>
@@ -76,18 +76,6 @@
   </si>
   <si>
     <t>Digikey</t>
-  </si>
-  <si>
-    <t>Harwin</t>
-  </si>
-  <si>
-    <t>FEMALE CRIMP CONTACT TIN LOOSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 952-2159-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> M20-1180046</t>
   </si>
   <si>
     <t>SFH11-PBPC-D25-ST-BK</t>
@@ -1019,11 +1007,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,7 +1062,7 @@
         <v>10</v>
       </c>
       <c r="K1" s="10">
-        <f>SUM(J2:J68)</f>
+        <f>SUM(J2:J67)</f>
         <v>44.970000000000006</v>
       </c>
     </row>
@@ -1083,16 +1071,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F2" s="13">
         <v>4</v>
@@ -1101,7 +1089,7 @@
         <v>18</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="I2" s="14">
         <v>0.12</v>
@@ -1118,16 +1106,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="29" t="s">
-        <v>72</v>
-      </c>
       <c r="D3" s="29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F3" s="7">
         <v>4</v>
@@ -1136,7 +1124,7 @@
         <v>18</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I3" s="7">
         <v>0.11</v>
@@ -1149,20 +1137,20 @@
     </row>
     <row r="4" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
-        <f t="shared" ref="A4:A25" si="1">A3+1</f>
+        <f t="shared" ref="A4:A24" si="1">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F4" s="7">
         <v>1</v>
@@ -1171,7 +1159,7 @@
         <v>18</v>
       </c>
       <c r="H4" s="29" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I4" s="7">
         <v>0.18</v>
@@ -1188,16 +1176,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F5" s="7">
         <v>3</v>
@@ -1206,7 +1194,7 @@
         <v>18</v>
       </c>
       <c r="H5" s="29" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I5" s="7">
         <v>0.14000000000000001</v>
@@ -1223,16 +1211,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F6" s="7">
         <v>3</v>
@@ -1241,7 +1229,7 @@
         <v>18</v>
       </c>
       <c r="H6" s="29" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="I6" s="7">
         <v>0.14000000000000001</v>
@@ -1258,16 +1246,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C7" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="F7" s="7">
         <v>1</v>
@@ -1276,7 +1264,7 @@
         <v>18</v>
       </c>
       <c r="H7" s="29" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I7" s="7">
         <v>0.35</v>
@@ -1293,16 +1281,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F8" s="7">
         <v>2</v>
@@ -1311,7 +1299,7 @@
         <v>18</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I8" s="20">
         <v>0.4</v>
@@ -1328,16 +1316,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C9" s="7">
         <v>3568</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F9" s="7">
         <v>2</v>
@@ -1346,7 +1334,7 @@
         <v>18</v>
       </c>
       <c r="H9" s="29" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I9" s="20">
         <v>0.98</v>
@@ -1363,16 +1351,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F10" s="7">
         <v>2</v>
@@ -1381,7 +1369,7 @@
         <v>18</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="I10" s="20">
         <v>0.47</v>
@@ -1398,16 +1386,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F11" s="7">
         <v>2</v>
@@ -1416,7 +1404,7 @@
         <v>18</v>
       </c>
       <c r="H11" s="29" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I11" s="20">
         <v>1.34</v>
@@ -1433,16 +1421,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F12" s="7">
         <v>2</v>
@@ -1451,7 +1439,7 @@
         <v>18</v>
       </c>
       <c r="H12" s="29" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="I12" s="20">
         <v>0.55000000000000004</v>
@@ -1471,13 +1459,13 @@
         <v>9</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F13" s="17">
         <v>2</v>
@@ -1486,7 +1474,7 @@
         <v>18</v>
       </c>
       <c r="H13" s="19" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="I13" s="22">
         <v>2.89</v>
@@ -1506,13 +1494,13 @@
         <v>17</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F14" s="7">
         <v>1</v>
@@ -1521,7 +1509,7 @@
         <v>18</v>
       </c>
       <c r="H14" s="29" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I14" s="7">
         <v>0.7</v>
@@ -1541,13 +1529,13 @@
         <v>17</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F15" s="7">
         <v>1</v>
@@ -1556,7 +1544,7 @@
         <v>18</v>
       </c>
       <c r="H15" s="29" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="I15" s="7">
         <v>1.01</v>
@@ -1573,16 +1561,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C16" s="29">
         <v>901303206</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F16" s="7">
         <v>6</v>
@@ -1591,7 +1579,7 @@
         <v>18</v>
       </c>
       <c r="H16" s="19" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I16" s="7">
         <v>1.55</v>
@@ -1608,16 +1596,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C17" s="29">
         <v>901420006</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F17" s="7">
         <f>F16</f>
@@ -1627,7 +1615,7 @@
         <v>18</v>
       </c>
       <c r="H17" s="19" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="I17" s="7">
         <v>0.43</v>
@@ -1644,13 +1632,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C18" s="29">
         <v>901190110</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E18" s="7" t="str">
         <f>E17</f>
@@ -1664,7 +1652,7 @@
         <v>18</v>
       </c>
       <c r="H18" s="19" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I18" s="7">
         <v>0.22</v>
@@ -1681,16 +1669,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F19" s="7">
         <v>1</v>
@@ -1699,7 +1687,7 @@
         <v>18</v>
       </c>
       <c r="H19" s="29" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="I19" s="20">
         <v>0.63</v>
@@ -1710,34 +1698,38 @@
       </c>
       <c r="K19" s="5"/>
     </row>
-    <row r="20" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B20" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
+      <c r="B20" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F20" s="7">
+        <v>6</v>
+      </c>
       <c r="G20" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="H20" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="I20" s="22">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="J20" s="21">
+      <c r="H20" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="I20" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="J20" s="18">
         <f>I20*F20</f>
-        <v>0</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="K20" s="5"/>
     </row>
@@ -1747,32 +1739,32 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>58</v>
+        <v>82</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>83</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="F21" s="7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G21" s="17" t="s">
         <v>18</v>
       </c>
       <c r="H21" s="29" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="I21" s="20">
         <v>0.1</v>
       </c>
       <c r="J21" s="18">
         <f>I21*F21</f>
-        <v>0.60000000000000009</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="K21" s="5"/>
     </row>
@@ -1782,152 +1774,116 @@
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" s="29" t="s">
-        <v>87</v>
+        <v>15</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>89</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F22" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G22" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="H22" s="29" t="s">
-        <v>88</v>
+      <c r="H22" s="30" t="s">
+        <v>91</v>
       </c>
       <c r="I22" s="20">
-        <v>0.1</v>
+        <v>0.78</v>
       </c>
       <c r="J22" s="18">
         <f>I22*F22</f>
-        <v>0.30000000000000004</v>
+        <v>1.56</v>
       </c>
       <c r="K22" s="5"/>
     </row>
-    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="16">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="30" t="s">
+      <c r="B23" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="17">
+        <v>1</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="22">
+        <v>0.49</v>
+      </c>
+      <c r="J23" s="21">
+        <f t="shared" ref="J23" si="6">I23*F23</f>
+        <v>0.49</v>
+      </c>
+      <c r="K23" s="5"/>
+    </row>
+    <row r="24" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="23">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="D23" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="E23" s="7" t="s">
+      <c r="D24" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="E24" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="24">
+        <v>1</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="F23" s="7">
-        <v>2</v>
-      </c>
-      <c r="G23" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="I23" s="20">
-        <v>0.78</v>
-      </c>
-      <c r="J23" s="18">
-        <f>I23*F23</f>
-        <v>1.56</v>
-      </c>
-      <c r="K23" s="5"/>
-    </row>
-    <row r="24" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="16">
-        <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="17">
-        <v>1</v>
-      </c>
-      <c r="G24" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="H24" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="I24" s="22">
-        <v>0.49</v>
-      </c>
-      <c r="J24" s="21">
-        <f t="shared" ref="J24" si="6">I24*F24</f>
-        <v>0.49</v>
+      <c r="I24" s="26">
+        <v>4.33</v>
+      </c>
+      <c r="J24" s="27">
+        <f t="shared" ref="J24" si="7">I24*F24</f>
+        <v>4.33</v>
       </c>
       <c r="K24" s="5"/>
     </row>
-    <row r="25" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="23">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="B25" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="C25" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="D25" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="E25" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" s="24">
-        <v>1</v>
-      </c>
-      <c r="G25" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="H25" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="I25" s="26">
-        <v>4.33</v>
-      </c>
-      <c r="J25" s="27">
-        <f t="shared" ref="J25" si="7">I25*F25</f>
-        <v>4.33</v>
-      </c>
-      <c r="K25" s="5"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G27" s="6"/>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G26" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H20" r:id="rId1"/>
-    <hyperlink ref="H13" r:id="rId2"/>
-    <hyperlink ref="H24" r:id="rId3"/>
-    <hyperlink ref="H8" r:id="rId4" display="BAT42CT-ND"/>
-    <hyperlink ref="H16" r:id="rId5" display=" WM8275-ND"/>
+    <hyperlink ref="H13" r:id="rId1"/>
+    <hyperlink ref="H23" r:id="rId2"/>
+    <hyperlink ref="H8" r:id="rId3" display="BAT42CT-ND"/>
+    <hyperlink ref="H16" r:id="rId4" display=" WM8275-ND"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updating board -- no DRC errors
</commit_message>
<xml_diff>
--- a/dwg/roboCoolerBOM.xlsx
+++ b/dwg/roboCoolerBOM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="113">
   <si>
     <t>Item</t>
   </si>
@@ -346,12 +346,24 @@
   </si>
   <si>
     <t>P7 P8 P10 P11 P13 P14</t>
+  </si>
+  <si>
+    <t>TL3342F160QG/TR</t>
+  </si>
+  <si>
+    <t>SWITCH TACTILE SPST-NO 0.05A 12V</t>
+  </si>
+  <si>
+    <t>EG2531CT-ND</t>
+  </si>
+  <si>
+    <t>E-Switch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
@@ -427,7 +439,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -609,6 +621,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -617,7 +651,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -700,6 +734,18 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -796,6 +842,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -831,6 +894,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1010,8 +1090,8 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,7 +1143,7 @@
       </c>
       <c r="K1" s="10">
         <f>SUM(J2:J67)</f>
-        <v>44.970000000000006</v>
+        <v>45.600000000000009</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -1137,7 +1217,7 @@
     </row>
     <row r="4" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
-        <f t="shared" ref="A4:A24" si="1">A3+1</f>
+        <f t="shared" ref="A4:A25" si="1">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
@@ -1868,10 +1948,41 @@
         <v>4.33</v>
       </c>
       <c r="J24" s="27">
-        <f t="shared" ref="J24" si="7">I24*F24</f>
+        <f t="shared" ref="J24:J25" si="7">I24*F24</f>
         <v>4.33</v>
       </c>
       <c r="K24" s="5"/>
+    </row>
+    <row r="25" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="23">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="F25" s="24">
+        <v>1</v>
+      </c>
+      <c r="G25" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="I25" s="34">
+        <v>0.63</v>
+      </c>
+      <c r="J25" s="35">
+        <f t="shared" si="7"/>
+        <v>0.63</v>
+      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G26" s="6"/>

</xml_diff>